<commit_message>
Update: Performer bearbeitet, Dispatcher und E-Mail Prozess hinzugefügt
</commit_message>
<xml_diff>
--- a/Performer/Data/Config.xlsx
+++ b/Performer/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MartinPrigge\Documents\UiPath\BCH_Queue_Framework\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timotheus.vrettos\develop\develop_RPA\uipath-rpa_lob\Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFBC8510-2C96-4F10-96FE-B089BA47EB45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A34C722E-E66E-419E-BBA6-A469852E1C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-2520" yWindow="-13050" windowWidth="16020" windowHeight="11325" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="83">
   <si>
     <t>Name</t>
   </si>
@@ -85,9 +85,6 @@
   </si>
   <si>
     <t>logF_BusinessProcessName</t>
-  </si>
-  <si>
-    <t>Framework</t>
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
@@ -159,9 +156,6 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>ProcessABCQueue</t>
-  </si>
-  <si>
     <t>MaxInitRetryNumber</t>
   </si>
   <si>
@@ -229,6 +223,57 @@
   </si>
   <si>
     <t>Utility path for saving temporary files. If left empty or not rooted a default folder is set . Will be deleted at end.</t>
+  </si>
+  <si>
+    <t>rpa001_WilmaTelephonebookLink</t>
+  </si>
+  <si>
+    <t>rpa001_InputFolderPath</t>
+  </si>
+  <si>
+    <t>rpa001_inProgressFolderPath</t>
+  </si>
+  <si>
+    <t>rpa001_FailedFolderPath</t>
+  </si>
+  <si>
+    <t>rpa001_DataFolderPath</t>
+  </si>
+  <si>
+    <t>rpa001_OutputFolderPath</t>
+  </si>
+  <si>
+    <t>rpa001_InputExcelFileName</t>
+  </si>
+  <si>
+    <t>rpa001_InputExcelSheetName</t>
+  </si>
+  <si>
+    <t>rpa001_EmailBodyHtmlPath</t>
+  </si>
+  <si>
+    <t>rpa001_EmailSubjetctLine</t>
+  </si>
+  <si>
+    <t>rpa001_Send_Groupmailbox</t>
+  </si>
+  <si>
+    <t>rpa001_StatusEmailReceiver</t>
+  </si>
+  <si>
+    <t>rpa001_EmailSmtpServer</t>
+  </si>
+  <si>
+    <t>rpa001_EmailSmtpPort</t>
+  </si>
+  <si>
+    <t>rpa001_LoB_Queue</t>
+  </si>
+  <si>
+    <t>Test/ITM/rpa001_LOB</t>
+  </si>
+  <si>
+    <t>rpa001_LoB_Bescheide</t>
   </si>
 </sst>
 </file>
@@ -280,7 +325,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -291,6 +336,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -309,9 +355,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -349,7 +395,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -455,7 +501,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -597,7 +643,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -608,15 +654,15 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -655,34 +701,38 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>23</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>80</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="4" t="s">
-        <v>32</v>
-      </c>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="30">
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="B4" s="5"/>
+    </row>
+    <row r="5" spans="1:26" ht="28.8">
       <c r="A5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" t="s">
-        <v>21</v>
+      <c r="B5" s="5" t="s">
+        <v>82</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1689,16 +1739,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1735,7 +1785,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1743,46 +1793,46 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="30">
+    <row r="3" spans="1:26" ht="28.8">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="45">
+    <row r="4" spans="1:26" ht="43.2">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:26" s="5" customFormat="1">
+    <row r="5" spans="1:26" s="5" customFormat="1" ht="14.4">
       <c r="A5" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1796,71 +1846,71 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:26" s="5" customFormat="1">
+    <row r="9" spans="1:26" s="5" customFormat="1" ht="14.4">
       <c r="A9" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B9" s="5">
         <v>0</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" s="5" customFormat="1" ht="14.4"/>
+    <row r="11" spans="1:26" s="5" customFormat="1" ht="14.4">
+      <c r="A11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" s="5" customFormat="1" ht="14.4">
+      <c r="A12" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" s="5" customFormat="1" ht="14.4">
+      <c r="A13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:26" s="5" customFormat="1"/>
-    <row r="11" spans="1:26" s="5" customFormat="1">
-      <c r="A11" t="s">
-        <v>50</v>
-      </c>
-      <c r="B11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" t="s">
-        <v>61</v>
+    <row r="14" spans="1:26" s="5" customFormat="1" ht="14.4">
+      <c r="A14" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:26" s="5" customFormat="1">
-      <c r="A12" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" s="5" customFormat="1">
-      <c r="A13" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" s="5" customFormat="1">
-      <c r="A14" s="5" t="s">
+    <row r="15" spans="1:26" s="5" customFormat="1" ht="14.4">
+      <c r="A15" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B15" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" s="5" customFormat="1">
-      <c r="A15" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1872,7 +1922,7 @@
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
@@ -1894,7 +1944,7 @@
         <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
@@ -1905,7 +1955,7 @@
         <v>17</v>
       </c>
       <c r="C20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
@@ -1916,53 +1966,53 @@
         <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B24">
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B25">
         <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:3" ht="45">
+    <row r="27" spans="1:3" ht="28.8">
       <c r="A27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B27" t="b">
         <v>0</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2945,16 +2995,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2965,7 +3015,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -2993,20 +3043,118 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>

</xml_diff>